<commit_message>
before intro to R
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">3 окт</t>
   </si>
   <si>
-    <t xml:space="preserve">Краткое введение в мир матричной алгебры</t>
+    <t xml:space="preserve">Краткое введение в мир линейной алгебры</t>
   </si>
   <si>
     <t xml:space="preserve">7 окт</t>
@@ -450,8 +450,8 @@
   </sheetPr>
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W12" activeCellId="0" sqref="W12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U10" activeCellId="0" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>